<commit_message>
fix bug when using budget() or budget2(), spreadsheet imported hol is ignored
</commit_message>
<xml_diff>
--- a/inst/exdata/sampleData.xlsx
+++ b/inst/exdata/sampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" state="visible" r:id="rId2"/>
@@ -212,27 +212,24 @@
     <t xml:space="preserve">Special</t>
   </si>
   <si>
-    <t xml:space="preserve">New Year's Day - additional</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chinese New Year</t>
   </si>
   <si>
     <t xml:space="preserve">EDSA People Power Revolution Anniversary</t>
   </si>
   <si>
+    <t xml:space="preserve">Maundy Thursday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Saturday</t>
+  </si>
+  <si>
     <t xml:space="preserve">Araw ng Kagitingan</t>
   </si>
   <si>
-    <t xml:space="preserve">Maundy Thursday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good Friday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black Saturday</t>
-  </si>
-  <si>
     <t xml:space="preserve">Labor Day</t>
   </si>
   <si>
@@ -242,12 +239,12 @@
     <t xml:space="preserve">Independence Day</t>
   </si>
   <si>
+    <t xml:space="preserve">Eid'l Fitr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adlaw ng Surigao del Norte</t>
   </si>
   <si>
-    <t xml:space="preserve">Eid'l Fitr</t>
-  </si>
-  <si>
     <t xml:space="preserve">Negotiated</t>
   </si>
   <si>
@@ -257,22 +254,25 @@
     <t xml:space="preserve">Ninoy Aquino Day</t>
   </si>
   <si>
+    <t xml:space="preserve">Eid'l Adha</t>
+  </si>
+  <si>
     <t xml:space="preserve">National Heroes Day</t>
   </si>
   <si>
-    <t xml:space="preserve">Eid'l Adha</t>
-  </si>
-  <si>
     <t xml:space="preserve">Araw ng Claver</t>
   </si>
   <si>
-    <t xml:space="preserve">Additional special (non-working day)</t>
-  </si>
-  <si>
     <t xml:space="preserve">All Saint's Day</t>
   </si>
   <si>
+    <t xml:space="preserve">All Soul’s Day</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bonifacio Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day Before Christmas</t>
   </si>
   <si>
     <t xml:space="preserve">Christmas Day</t>
@@ -397,8 +397,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -831,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -874,10 +874,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>61</v>
@@ -888,10 +888,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>61</v>
@@ -902,13 +902,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>64</v>
@@ -916,10 +916,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>59</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>66</v>
@@ -947,7 +947,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>59</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>68</v>
@@ -975,10 +975,10 @@
         <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>69</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>70</v>
@@ -1003,7 +1003,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>59</v>
@@ -1028,27 +1028,27 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>75</v>
@@ -1059,10 +1059,10 @@
         <v>18</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>76</v>
@@ -1073,7 +1073,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
@@ -1087,10 +1087,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>78</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>79</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>61</v>
@@ -1129,10 +1129,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>81</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
introduce slot dcc (dump cost code) in Employee-class
</commit_message>
<xml_diff>
--- a/inst/exdata/sampleData.xlsx
+++ b/inst/exdata/sampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="88">
   <si>
     <t xml:space="preserve">activity</t>
   </si>
@@ -59,6 +59,12 @@
     <t xml:space="preserve">Clerk</t>
   </si>
   <si>
+    <t xml:space="preserve">Materials Handling General2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14100</t>
+  </si>
+  <si>
     <t xml:space="preserve">January</t>
   </si>
   <si>
@@ -125,6 +131,18 @@
     <t xml:space="preserve">isRF</t>
   </si>
   <si>
+    <t xml:space="preserve">d.rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc</t>
+  </si>
+  <si>
     <t xml:space="preserve">S-240</t>
   </si>
   <si>
@@ -140,9 +158,6 @@
     <t xml:space="preserve">reg</t>
   </si>
   <si>
-    <t xml:space="preserve">2012-10-15</t>
-  </si>
-  <si>
     <t xml:space="preserve">TRUE</t>
   </si>
   <si>
@@ -161,9 +176,6 @@
     <t xml:space="preserve">Materials Handling Office Clerk</t>
   </si>
   <si>
-    <t xml:space="preserve">2013-08-16</t>
-  </si>
-  <si>
     <t xml:space="preserve">10-168</t>
   </si>
   <si>
@@ -173,19 +185,10 @@
     <t xml:space="preserve">MH Clerk</t>
   </si>
   <si>
-    <t xml:space="preserve">2016-08-13</t>
-  </si>
-  <si>
     <t xml:space="preserve">E-0001</t>
   </si>
   <si>
     <t xml:space="preserve">sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-01-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-12-31</t>
   </si>
   <si>
     <t xml:space="preserve">E-0002</t>
@@ -291,10 +294,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="MM/DD/YYYY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -361,7 +365,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -375,6 +379,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -395,10 +407,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -471,7 +483,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
@@ -481,6 +493,29 @@
       </c>
       <c r="G3" s="1" t="n">
         <v>14000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -499,10 +534,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -516,45 +551,50 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -573,10 +613,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -593,19 +633,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -614,36 +654,48 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -652,30 +704,30 @@
         <v>14000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>41197</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -687,30 +739,30 @@
         <v>14000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>41502</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
@@ -722,30 +774,30 @@
         <v>14000</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>42595</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -757,33 +809,33 @@
         <v>14000</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>43101</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>43465</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -795,22 +847,22 @@
         <v>14000</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>43101</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>43465</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -831,7 +883,7 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -846,352 +898,352 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>15</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>13</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>25</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>31</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1223,15 +1275,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>20000</v>
@@ -1239,7 +1291,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20000</v>
@@ -1247,7 +1299,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>400</v>
@@ -1255,7 +1307,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>400</v>
@@ -1263,7 +1315,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>20000</v>

</xml_diff>

<commit_message>
include forecast argument in budget()
</commit_message>
<xml_diff>
--- a/inst/exdata/sampleData.xlsx
+++ b/inst/exdata/sampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t xml:space="preserve">activity</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">dcc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field</t>
   </si>
   <si>
     <t xml:space="preserve">S-240</t>
@@ -409,7 +412,7 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -613,10 +616,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R7" activeCellId="0" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -683,19 +686,22 @@
       <c r="Q1" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -704,30 +710,33 @@
         <v>14000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I2" s="5" t="n">
         <v>41197</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -739,30 +748,33 @@
         <v>14000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I3" s="5" t="n">
         <v>41502</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
@@ -774,30 +786,33 @@
         <v>14000</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I4" s="5" t="n">
         <v>42595</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>44</v>
+      <c r="R4" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -809,7 +824,7 @@
         <v>14000</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>43101</v>
@@ -818,24 +833,27 @@
         <v>43465</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>44</v>
+      <c r="R5" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -847,7 +865,7 @@
         <v>14000</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>43101</v>
@@ -856,13 +874,16 @@
         <v>43465</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M6" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -898,16 +919,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -918,10 +939,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,10 +953,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,10 +967,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -960,10 +981,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,10 +995,10 @@
         <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,10 +1009,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1002,10 +1023,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,10 +1037,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,10 +1051,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,10 +1065,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,10 +1079,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,10 +1093,10 @@
         <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,10 +1107,10 @@
         <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,10 +1121,10 @@
         <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1114,10 +1135,10 @@
         <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1128,10 +1149,10 @@
         <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,10 +1163,10 @@
         <v>13</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,10 +1177,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,10 +1191,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1184,10 +1205,10 @@
         <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,10 +1219,10 @@
         <v>24</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,10 +1233,10 @@
         <v>25</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,10 +1247,10 @@
         <v>30</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1240,10 +1261,10 @@
         <v>31</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1278,12 +1299,12 @@
         <v>25</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>20000</v>
@@ -1291,7 +1312,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20000</v>
@@ -1299,7 +1320,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>400</v>
@@ -1307,7 +1328,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>400</v>
@@ -1315,7 +1336,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>20000</v>

</xml_diff>

<commit_message>
add dependents in Employee slots
</commit_message>
<xml_diff>
--- a/inst/exdata/sampleData.xlsx
+++ b/inst/exdata/sampleData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="101">
   <si>
     <t xml:space="preserve">activity</t>
   </si>
@@ -110,6 +110,9 @@
     <t xml:space="preserve">designation</t>
   </si>
   <si>
+    <t xml:space="preserve">field</t>
+  </si>
+  <si>
     <t xml:space="preserve">attendance</t>
   </si>
   <si>
@@ -131,6 +134,42 @@
     <t xml:space="preserve">isRF</t>
   </si>
   <si>
+    <t xml:space="preserve">JAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC</t>
+  </si>
+  <si>
     <t xml:space="preserve">d.rd</t>
   </si>
   <si>
@@ -143,9 +182,6 @@
     <t xml:space="preserve">dcc</t>
   </si>
   <si>
-    <t xml:space="preserve">field</t>
-  </si>
-  <si>
     <t xml:space="preserve">S-240</t>
   </si>
   <si>
@@ -158,10 +194,10 @@
     <t xml:space="preserve">Section Head</t>
   </si>
   <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
     <t xml:space="preserve">reg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
   </si>
   <si>
     <t xml:space="preserve">Sunday</t>
@@ -616,10 +652,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R7" activeCellId="0" sqref="R7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -628,10 +664,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="12.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="12.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="30" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="32" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,21 +689,21 @@
         <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -674,13 +712,13 @@
       <c r="M1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q1" s="1" t="s">
@@ -689,201 +727,417 @@
       <c r="R1" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>14000</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="5" t="n">
         <v>41197</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="n">
+      <c r="E3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>14000</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="5" t="n">
         <v>41502</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="n">
+      <c r="E4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>14000</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="5" t="n">
         <v>42595</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="n">
+      <c r="E5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>14000</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="5" t="n">
         <v>43101</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="K5" s="5" t="n">
         <v>43465</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="n">
+      <c r="E6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>14000</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="5" t="n">
+      <c r="I6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="5" t="n">
         <v>43101</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="K6" s="5" t="n">
         <v>43465</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -919,16 +1173,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,10 +1193,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,10 +1207,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,10 +1221,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -981,10 +1235,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,10 +1249,10 @@
         <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,10 +1263,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,10 +1277,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,10 +1291,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1051,10 +1305,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,10 +1319,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1079,10 +1333,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,10 +1347,10 @@
         <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,10 +1361,10 @@
         <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1121,10 +1375,10 @@
         <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1135,10 +1389,10 @@
         <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,10 +1403,10 @@
         <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1163,10 +1417,10 @@
         <v>13</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,10 +1431,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,10 +1445,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1205,10 +1459,10 @@
         <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,10 +1473,10 @@
         <v>24</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,10 +1487,10 @@
         <v>25</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,10 +1501,10 @@
         <v>30</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,10 +1515,10 @@
         <v>31</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1299,12 +1553,12 @@
         <v>25</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>20000</v>
@@ -1312,7 +1566,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20000</v>
@@ -1320,7 +1574,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>400</v>
@@ -1328,7 +1582,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>400</v>
@@ -1336,7 +1590,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>20000</v>

</xml_diff>

<commit_message>
initial importation of VL/SL
Not yet used in object assignment.
</commit_message>
<xml_diff>
--- a/inst/exdata/sampleData.xlsx
+++ b/inst/exdata/sampleData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="116">
   <si>
     <t xml:space="preserve">activity</t>
   </si>
@@ -215,6 +215,12 @@
     <t xml:space="preserve">a_12</t>
   </si>
   <si>
+    <t xml:space="preserve">VL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SL</t>
+  </si>
+  <si>
     <t xml:space="preserve">S-240</t>
   </si>
   <si>
@@ -237,6 +243,9 @@
   </si>
   <si>
     <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">S-156</t>
@@ -485,16 +494,16 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="AP1:AQ6 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="8" style="1" width="11.57"/>
@@ -611,10 +620,10 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="AP1:AQ6 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
   </cols>
@@ -686,10 +695,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO6"/>
+  <dimension ref="A1:AQ6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO3" activeCellId="0" sqref="AO3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AP1" activeCellId="0" sqref="AP1:AQ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -829,40 +838,46 @@
       <c r="AO1" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="AP1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I2" s="5" t="n">
         <v>41197</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="N2" s="1" t="n">
         <v>1</v>
@@ -935,41 +950,47 @@
       </c>
       <c r="AO2" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I3" s="5" t="n">
         <v>41502</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="N3" s="1" t="n">
         <v>1</v>
@@ -1042,42 +1063,48 @@
       </c>
       <c r="AO3" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I4" s="5" t="n">
         <v>42595</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="N4" s="1" t="n">
         <v>1</v>
       </c>
@@ -1149,29 +1176,35 @@
       </c>
       <c r="AO4" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>43101</v>
@@ -1180,14 +1213,14 @@
         <v>43465</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="N5" s="1" t="n">
         <v>1</v>
       </c>
@@ -1259,29 +1292,35 @@
       </c>
       <c r="AO5" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="AP5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>43101</v>
@@ -1290,13 +1329,13 @@
         <v>43465</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="N6" s="1" t="n">
         <v>1</v>
@@ -1369,6 +1408,12 @@
       </c>
       <c r="AO6" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="AP6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1390,29 +1435,29 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="1" sqref="AP1:AQ6 I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1423,10 +1468,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1437,10 +1482,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,10 +1496,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,10 +1510,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1479,10 +1524,10 @@
         <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,10 +1538,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1507,10 +1552,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1521,10 +1566,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,10 +1580,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,10 +1594,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,10 +1608,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1577,10 +1622,10 @@
         <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,10 +1636,10 @@
         <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,10 +1650,10 @@
         <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,10 +1664,10 @@
         <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,10 +1678,10 @@
         <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,10 +1692,10 @@
         <v>13</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1661,10 +1706,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1675,10 +1720,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,10 +1734,10 @@
         <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,10 +1748,10 @@
         <v>24</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,10 +1762,10 @@
         <v>25</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,10 +1776,10 @@
         <v>30</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,10 +1790,10 @@
         <v>31</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1770,25 +1815,25 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="AP1:AQ6 C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>20000</v>
@@ -1799,7 +1844,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20000</v>
@@ -1810,7 +1855,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>400</v>
@@ -1821,7 +1866,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>400</v>
@@ -1832,7 +1877,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>20000</v>

</xml_diff>

<commit_message>
make overtime days adjustment per month
</commit_message>
<xml_diff>
--- a/inst/exdata/sampleData.xlsx
+++ b/inst/exdata/sampleData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="149">
   <si>
     <t xml:space="preserve">activity</t>
   </si>
@@ -167,16 +167,131 @@
     <t xml:space="preserve">DEC</t>
   </si>
   <si>
-    <t xml:space="preserve">d.rd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d.ho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d.rh</t>
-  </si>
-  <si>
     <t xml:space="preserve">dcc</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">d.rd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rd_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.ho_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.rh_12</t>
   </si>
   <si>
     <t xml:space="preserve">a_1</t>
@@ -384,7 +499,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -405,6 +520,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -449,7 +569,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -464,6 +584,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -494,7 +618,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="AP1:AQ6 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -620,10 +744,10 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="AP1:AQ6 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
   </cols>
@@ -695,10 +819,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AQ6"/>
+  <dimension ref="A1:BX6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AP1" activeCellId="0" sqref="AP1:AQ6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z1" activeCellId="0" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -710,8 +834,14 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="13.02"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="29" min="11" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="31" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="11" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="11.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="38" min="28" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="11.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="50" min="40" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="11.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="62" min="52" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="64" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,19 +920,19 @@
       <c r="Y1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="AA1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="AE1" s="1" t="s">
@@ -829,55 +959,154 @@
       <c r="AL1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>64</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="BE1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="BK1" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="5" t="n">
+        <v>103</v>
+      </c>
+      <c r="I2" s="6" t="n">
         <v>41197</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="N2" s="1" t="n">
         <v>1</v>
@@ -915,82 +1144,82 @@
       <c r="Y2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AD2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>73</v>
+      <c r="BK2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BU2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BX2" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="5" t="n">
+        <v>103</v>
+      </c>
+      <c r="I3" s="6" t="n">
         <v>41502</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="N3" s="1" t="n">
         <v>1</v>
@@ -1028,82 +1257,82 @@
       <c r="Y3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AD3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>73</v>
+      <c r="BK3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BU3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BX3" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" s="5" t="n">
+        <v>103</v>
+      </c>
+      <c r="I4" s="6" t="n">
         <v>42595</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>1</v>
@@ -1141,85 +1370,85 @@
       <c r="Y4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AD4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
-        <v>73</v>
+      <c r="BK4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BU4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BX4" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I5" s="5" t="n">
+        <v>114</v>
+      </c>
+      <c r="I5" s="6" t="n">
         <v>43101</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="6" t="n">
         <v>43465</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>1</v>
@@ -1257,85 +1486,85 @@
       <c r="Y5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AD5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ5" s="1" t="s">
-        <v>73</v>
+      <c r="BK5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BU5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BX5" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I6" s="5" t="n">
+        <v>114</v>
+      </c>
+      <c r="I6" s="6" t="n">
         <v>43101</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" s="6" t="n">
         <v>43465</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="N6" s="1" t="n">
         <v>1</v>
@@ -1373,47 +1602,47 @@
       <c r="Y6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AD6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ6" s="1" t="s">
-        <v>73</v>
+      <c r="BK6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BU6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BX6" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1435,10 +1664,10 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="1" sqref="AP1:AQ6 I19"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.71"/>
@@ -1448,16 +1677,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,10 +1697,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,10 +1711,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,10 +1725,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,10 +1739,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,10 +1753,10 @@
         <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,10 +1767,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>94</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,10 +1781,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,10 +1795,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,10 +1809,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,10 +1823,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,10 +1837,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,10 +1851,10 @@
         <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,10 +1865,10 @@
         <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,10 +1879,10 @@
         <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,10 +1893,10 @@
         <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,10 +1907,10 @@
         <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,10 +1921,10 @@
         <v>13</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,10 +1935,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,10 +1949,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,10 +1963,10 @@
         <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,10 +1977,10 @@
         <v>24</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,10 +1991,10 @@
         <v>25</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,10 +2005,10 @@
         <v>30</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,10 +2019,10 @@
         <v>31</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1815,25 +2044,25 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="AP1:AQ6 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>20000</v>
@@ -1844,7 +2073,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20000</v>
@@ -1855,7 +2084,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>400</v>
@@ -1866,7 +2095,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>400</v>
@@ -1877,7 +2106,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>20000</v>

</xml_diff>

<commit_message>
rename cost code to cost center
fixes #3
</commit_message>
<xml_diff>
--- a/inst/exdata/sampleData.xlsx
+++ b/inst/exdata/sampleData.xlsx
@@ -44,7 +44,7 @@
     <t xml:space="preserve">OT</t>
   </si>
   <si>
-    <t xml:space="preserve">costCode</t>
+    <t xml:space="preserve">costCenter</t>
   </si>
   <si>
     <t xml:space="preserve">Materials Handling General</t>
@@ -170,23 +170,7 @@
     <t xml:space="preserve">dcc</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">d.rd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_1</t>
-    </r>
+    <t xml:space="preserve">d.rd_1</t>
   </si>
   <si>
     <t xml:space="preserve">d.rd_2</t>
@@ -499,7 +483,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -520,11 +504,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -569,7 +548,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -584,10 +563,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -618,7 +593,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -747,7 +722,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
   </cols>
@@ -821,8 +796,8 @@
   </sheetPr>
   <dimension ref="A1:BX6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z1" activeCellId="0" sqref="Z1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -959,76 +934,76 @@
       <c r="AL1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AM1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AN1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AO1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AP1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AR1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AS1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AT1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AU1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AV1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AW1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AX1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AY1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BA1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BB1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BC1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BD1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BE1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BF1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BG1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BH1" s="5" t="s">
+      <c r="BH1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BI1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BJ1" s="5" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>83</v>
       </c>
       <c r="BK1" s="0" t="s">
@@ -1096,7 +1071,7 @@
       <c r="H2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="5" t="n">
         <v>41197</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -1209,7 +1184,7 @@
       <c r="H3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="6" t="n">
+      <c r="I3" s="5" t="n">
         <v>41502</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -1322,7 +1297,7 @@
       <c r="H4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="5" t="n">
         <v>42595</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -1435,10 +1410,10 @@
       <c r="H5" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="5" t="n">
         <v>43101</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="J5" s="5" t="n">
         <v>43465</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -1551,10 +1526,10 @@
       <c r="H6" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I6" s="5" t="n">
         <v>43101</v>
       </c>
-      <c r="J6" s="6" t="n">
+      <c r="J6" s="5" t="n">
         <v>43465</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -1667,7 +1642,7 @@
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.71"/>
@@ -2047,7 +2022,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
enable having a different dump cost center for every month
fixes #10
</commit_message>
<xml_diff>
--- a/inst/exdata/sampleData.xlsx
+++ b/inst/exdata/sampleData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="160">
   <si>
     <t xml:space="preserve">activity</t>
   </si>
@@ -167,7 +167,40 @@
     <t xml:space="preserve">DEC</t>
   </si>
   <si>
-    <t xml:space="preserve">dcc</t>
+    <t xml:space="preserve">dcc_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcc_12</t>
   </si>
   <si>
     <t xml:space="preserve">d.rd_1</t>
@@ -722,7 +755,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
   </cols>
@@ -794,10 +827,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BX6"/>
+  <dimension ref="A1:CI6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AK1" activeCellId="0" sqref="AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -811,12 +844,14 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="11" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="11.59"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="38" min="28" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="11.59"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="50" min="40" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="11.59"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="62" min="52" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="64" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="37" min="28" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="11.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="49" min="39" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="11.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="61" min="51" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="62" min="62" style="1" width="11.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="73" min="63" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="75" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -898,7 +933,7 @@
       <c r="Z1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="1" t="s">
         <v>48</v>
       </c>
       <c r="AB1" s="1" t="s">
@@ -931,40 +966,40 @@
       <c r="AK1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="AX1" s="4" t="s">
@@ -1006,40 +1041,40 @@
       <c r="BJ1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BK1" s="0" t="s">
+      <c r="BK1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BL1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BM1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BN1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BO1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BP1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BR1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BS1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BT1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BU1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BV1" s="0" t="s">
         <v>95</v>
       </c>
       <c r="BW1" s="1" t="s">
@@ -1048,40 +1083,73 @@
       <c r="BX1" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="BY1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="I2" s="5" t="n">
         <v>41197</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="N2" s="1" t="n">
         <v>1</v>
@@ -1119,82 +1187,82 @@
       <c r="Y2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BK2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BQ2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BR2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BS2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BT2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU2" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="BV2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BW2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BX2" s="1" t="s">
-        <v>106</v>
+      <c r="BW2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CE2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CG2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CI2" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="I3" s="5" t="n">
         <v>41502</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="N3" s="1" t="n">
         <v>1</v>
@@ -1232,82 +1300,82 @@
       <c r="Y3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BK3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BQ3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BR3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BS3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BT3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU3" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="BV3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BW3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BX3" s="1" t="s">
-        <v>106</v>
+      <c r="BW3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CE3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CG3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CI3" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="I4" s="5" t="n">
         <v>42595</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>1</v>
@@ -1345,70 +1413,70 @@
       <c r="Y4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BK4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BQ4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BR4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BS4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BT4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU4" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="BV4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BW4" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BX4" s="1" t="s">
-        <v>106</v>
+      <c r="BW4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CE4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CG4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CI4" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>43101</v>
@@ -1417,13 +1485,13 @@
         <v>43465</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>1</v>
@@ -1461,70 +1529,70 @@
       <c r="Y5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BK5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BQ5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BR5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BS5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BT5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU5" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="BV5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BW5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BX5" s="1" t="s">
-        <v>106</v>
+      <c r="BW5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CE5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CG5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CI5" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>14000</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>43101</v>
@@ -1533,13 +1601,13 @@
         <v>43465</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="N6" s="1" t="n">
         <v>1</v>
@@ -1577,47 +1645,47 @@
       <c r="Y6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BK6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BQ6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BR6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BS6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BT6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU6" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="BV6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BW6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BX6" s="1" t="s">
-        <v>106</v>
+      <c r="BW6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CE6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CG6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CI6" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1642,7 +1710,7 @@
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.71"/>
@@ -1652,16 +1720,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,10 +1740,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,10 +1754,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1700,10 +1768,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,10 +1782,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,10 +1796,10 @@
         <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,10 +1810,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1756,10 +1824,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,10 +1838,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,10 +1852,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1798,10 +1866,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,10 +1880,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1826,10 +1894,10 @@
         <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1840,10 +1908,10 @@
         <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,10 +1922,10 @@
         <v>21</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,10 +1936,10 @@
         <v>22</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,10 +1950,10 @@
         <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,10 +1964,10 @@
         <v>13</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,10 +1978,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,10 +1992,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,10 +2006,10 @@
         <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,10 +2020,10 @@
         <v>24</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,10 +2034,10 @@
         <v>25</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,10 +2048,10 @@
         <v>30</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1994,10 +2062,10 @@
         <v>31</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2022,22 +2090,22 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>20000</v>
@@ -2048,7 +2116,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20000</v>
@@ -2059,7 +2127,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>400</v>
@@ -2070,7 +2138,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>400</v>
@@ -2081,7 +2149,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>20000</v>

</xml_diff>

<commit_message>
rename unclear dependents column
fixes #13
</commit_message>
<xml_diff>
--- a/inst/exdata/sampleData.xlsx
+++ b/inst/exdata/sampleData.xlsx
@@ -131,40 +131,40 @@
     <t xml:space="preserve">isRF</t>
   </si>
   <si>
-    <t xml:space="preserve">JAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JUN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JUL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEC</t>
+    <t xml:space="preserve">dependents_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependents_12</t>
   </si>
   <si>
     <t xml:space="preserve">dcc_1</t>
@@ -619,7 +619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -745,7 +745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -755,7 +755,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
   </cols>
@@ -823,14 +823,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:CI6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK1" activeCellId="0" sqref="AK1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -842,7 +842,12 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="13.02"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="11" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="11" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="14" style="1" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="13.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="11.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="37" min="28" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="11.59"/>
@@ -1700,7 +1705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1710,7 +1715,7 @@
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.71"/>
@@ -2080,7 +2085,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2090,7 +2095,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>